<commit_message>
Creating sample inventory table
</commit_message>
<xml_diff>
--- a/Sample inventory_tomatoes.xlsx
+++ b/Sample inventory_tomatoes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\em18yraw\Desktop\SI_SoSe2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\Stable-Isotope-Ratio-Analysis-of-Tomatoes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C529854E-15FD-4822-BC8D-7634C646E61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E018B6-4732-4A56-A5E5-2FF02DAF1AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{F2BF5F27-B057-432E-8C50-7FC9FB0FB91A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{F2BF5F27-B057-432E-8C50-7FC9FB0FB91A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample inventory" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -579,22 +579,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB55EAF-02FF-4209-94A8-EBA8FE383566}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.1796875" customWidth="1"/>
-    <col min="7" max="7" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" customWidth="1"/>
-    <col min="11" max="11" width="8.54296875" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -629,7 +631,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -664,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -696,10 +698,10 @@
         <v>16</v>
       </c>
       <c r="K3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -731,7 +733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -763,7 +765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -792,10 +794,10 @@
         <v>14</v>
       </c>
       <c r="K6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -827,7 +829,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -859,10 +861,10 @@
         <v>39</v>
       </c>
       <c r="K8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -897,7 +899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -929,10 +931,10 @@
         <v>42</v>
       </c>
       <c r="K10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -961,7 +963,7 @@
         <v>14</v>
       </c>
       <c r="K11">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>